<commit_message>
Task 50 - страница ошибки + settings : Production
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="126">
   <si>
     <t>Задача</t>
   </si>
@@ -436,6 +436,15 @@
   </si>
   <si>
     <t>Вызов плагина DataTable вне onReady , т.к. дергается экран при отрисовке стилей</t>
+  </si>
+  <si>
+    <t>Страница ошибки</t>
+  </si>
+  <si>
+    <t>Error.cshtml</t>
+  </si>
+  <si>
+    <t>task 50</t>
   </si>
 </sst>
 </file>
@@ -955,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2216,6 +2225,20 @@
         <v>122</v>
       </c>
     </row>
+    <row r="52" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K52" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2224,10 +2247,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2375,6 +2398,23 @@
         <v>121</v>
       </c>
       <c r="F11" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>